<commit_message>
metamiss updates - bug fixes for no obs and logimor(varname) help file - updated references, UCL email, added imor() test file - improved data - retrieved and reduced to the 17 studies do-file - created from help file (replaces previous do-file)
</commit_message>
<xml_diff>
--- a/metamiss-to-do.xlsx
+++ b/metamiss-to-do.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>DONE</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>If run with no data in memory, gives error about wrong metan version</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>now gives error if argument varies over observations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metamiss, logimor(varname) behaves like logimor(varname[1]) </t>
+  </si>
+  <si>
+    <t>enable metamiss, logimor(varname) [also other options]</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -442,7 +464,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:E3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,27 +509,52 @@
       <c r="C3" s="5">
         <v>43299</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7">
+        <v>43370</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>43284</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7">
+        <v>43370</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>43284</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="expression" dxfId="0" priority="13">
+  <conditionalFormatting sqref="A3:A4">
+    <cfRule type="expression" dxfId="2" priority="14">
       <formula>ISBLANK($E3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISBLANK($E5)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Improved help file using Ella's comments.
</commit_message>
<xml_diff>
--- a/metamiss-to-do.xlsx
+++ b/metamiss-to-do.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\metamiss\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8F4131-B775-4CE4-A0D9-C3BF4EE63DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15450" windowHeight="9690"/>
+    <workbookView xWindow="5145" yWindow="1605" windowWidth="18030" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,24 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>DONE</t>
   </si>
@@ -53,12 +71,81 @@
   </si>
   <si>
     <t>enable metamiss, logimor(varname) [also other options]</t>
+  </si>
+  <si>
+    <t>change gen to gen double to improve agreement with metan</t>
+  </si>
+  <si>
+    <t>'jump to' and 'also see' boxes</t>
+  </si>
+  <si>
+    <t>currently these are greyed out, would be good to have drop down options populated</t>
+  </si>
+  <si>
+    <t>Description (i)</t>
+  </si>
+  <si>
+    <t>Higgins et al. needs date.  Could also have hyperlink to reference later in helpfile</t>
+  </si>
+  <si>
+    <t>Description (ii)</t>
+  </si>
+  <si>
+    <t>White et al needs date as above.  References could be hyperlinked</t>
+  </si>
+  <si>
+    <t>Syntax</t>
+  </si>
+  <si>
+    <t>What are rE fE mE rC fC and mC ?</t>
+  </si>
+  <si>
+    <t>Imputation using reasons</t>
+  </si>
+  <si>
+    <t>What are mfE mfC mpE mpC ?</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>What are IMOR, ACA ?</t>
+  </si>
+  <si>
+    <t>Sometimes 'metan' is hyperlinked, sometimes just in bf.</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Julian Higgins, School of Social and Community Medicine, University of Bristol, UK.  But hyperlink for associated SJ to cite software has Julian at Cambridge.</t>
+  </si>
+  <si>
+    <t>AREA</t>
+  </si>
+  <si>
+    <t>Ella</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>explained</t>
+  </si>
+  <si>
+    <t>I think this is clear enough</t>
+  </si>
+  <si>
+    <t>citation gives correct affiliation when SJ article was written</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -93,26 +180,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -120,29 +192,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -157,6 +226,45 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -164,8 +272,26 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{85BA75C0-548F-408C-95A4-A8F4349F7199}" name="Table1" displayName="Table1" ref="A2:F14" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A2:F14" xr:uid="{85BA75C0-548F-408C-95A4-A8F4349F7199}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6D394D52-4989-46BB-92A3-670888AC6F51}" name="AREA" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{3560AF1C-3E00-4C39-9449-53F357725322}" name="TASK" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E93EB31F-683C-496F-927F-295F52C5239A}" name="FROM" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{139B4224-2524-4E5E-BA9A-5E92281E6DDD}" name="NOTED"/>
+    <tableColumn id="4" xr3:uid="{CBCEFB95-CD80-460B-A114-0B968FD7874C}" name="ACTION" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{07BE5E9F-DD43-4495-8B42-305641B483CD}" name="DONE" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -211,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,9 +370,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +422,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,107 +614,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="7">
         <v>43299</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="6">
         <v>43370</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="7">
         <v>43284</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="6">
         <v>43370</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D5" s="7">
         <v>43284</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>44697</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6">
+        <v>44697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7">
+        <v>44693</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="6">
+        <v>44697</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:A4">
-    <cfRule type="expression" dxfId="2" priority="14">
-      <formula>ISBLANK($E3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($E5)</formula>
+  <conditionalFormatting sqref="B3:B14">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK($F3)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -562,5 +899,8 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;F&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>